<commit_message>
binh dong, bavet, svayrieng
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JF.xlsx
+++ b/invoice_gen/TEMPLATE/JF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\gen_inv\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D8153-A0F3-4B8C-A7F1-112190F50816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798D18C3-E880-4B9D-B524-8AD677924DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t>SALES CONTRACT</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>FCA:</t>
-  </si>
-  <si>
-    <t>BINH PHUOC</t>
   </si>
   <si>
     <t>Term of Payment: 100% TT after shipment</t>
@@ -388,6 +385,12 @@
   <si>
     <t>JFINV</t>
   </si>
+  <si>
+    <t>BAVET, SVAYRIENG</t>
+  </si>
+  <si>
+    <t>BAVET, SVAY RIENG</t>
+  </si>
 </sst>
 </file>
 
@@ -400,7 +403,7 @@
     <numFmt numFmtId="166" formatCode="###0;###0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,12 +519,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -637,13 +634,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -706,11 +696,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -799,11 +789,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -813,44 +803,44 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="23" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="24" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="24" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -858,9 +848,6 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -870,17 +857,14 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -911,10 +895,10 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -935,9 +919,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -950,23 +934,35 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -983,23 +979,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1689,264 +1679,264 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" style="35" customWidth="1"/>
-    <col min="6" max="16381" width="28.7109375" style="35" customWidth="1"/>
-    <col min="16382" max="16384" width="28.7109375" style="35"/>
+    <col min="1" max="1" width="17.7109375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="34" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" style="34" customWidth="1"/>
+    <col min="6" max="16381" width="28.7109375" style="34" customWidth="1"/>
+    <col min="16382" max="16384" width="28.7109375" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45.95" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-    </row>
-    <row r="2" spans="1:5" s="36" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-    </row>
-    <row r="3" spans="1:5" s="36" customFormat="1" ht="27" customHeight="1">
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+    </row>
+    <row r="2" spans="1:5" s="35" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+    </row>
+    <row r="3" spans="1:5" s="35" customFormat="1" ht="27" customHeight="1">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="57" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="36" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
+      <c r="E3" s="56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="35" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="58" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="37" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A5" s="42" t="s">
+      <c r="E4" s="57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="37" customFormat="1" ht="32.1" customHeight="1">
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
+      <c r="B6" s="36" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="37" customFormat="1" ht="32.1" customHeight="1">
-      <c r="B7" s="37" t="s">
+    <row r="7" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
+      <c r="B7" s="36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="37" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-    </row>
-    <row r="9" spans="1:5" s="37" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A9" s="42" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="37" customFormat="1" ht="45" customHeight="1">
-      <c r="A10" s="42"/>
-      <c r="B10" s="92" t="s">
+    <row r="10" spans="1:5" s="36" customFormat="1" ht="45" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-    </row>
-    <row r="11" spans="1:5" s="37" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A11" s="42"/>
-      <c r="B11" s="92" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+    </row>
+    <row r="11" spans="1:5" s="36" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-    </row>
-    <row r="12" spans="1:5" s="37" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="95" t="s">
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+    </row>
+    <row r="12" spans="1:5" s="36" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="95"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="42"/>
-    </row>
-    <row r="13" spans="1:5" s="37" customFormat="1" ht="60.95" customHeight="1">
-      <c r="A13" s="92" t="s">
+      <c r="B12" s="93"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="41"/>
+    </row>
+    <row r="13" spans="1:5" s="36" customFormat="1" ht="60.95" customHeight="1">
+      <c r="A13" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-    </row>
-    <row r="14" spans="1:5" s="37" customFormat="1" ht="54.95" customHeight="1">
-      <c r="A14" s="93" t="s">
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+    </row>
+    <row r="14" spans="1:5" s="36" customFormat="1" ht="54.95" customHeight="1">
+      <c r="A14" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
     </row>
     <row r="15" spans="1:5" ht="15.75">
-      <c r="A15" s="45"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
     </row>
     <row r="16" spans="1:5" ht="27.95" customHeight="1">
-      <c r="A16" s="96"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-    </row>
-    <row r="17" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A17" s="46" t="s">
+      <c r="A16" s="94"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+    </row>
+    <row r="17" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A17" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+    </row>
+    <row r="18" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A18" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-    </row>
-    <row r="18" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A18" s="42" t="s">
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A19" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-    </row>
-    <row r="19" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A19" s="42" t="s">
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+    </row>
+    <row r="20" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A20" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-    </row>
-    <row r="20" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A20" s="42" t="s">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+    </row>
+    <row r="21" spans="1:6" s="36" customFormat="1" ht="45.95" customHeight="1">
+      <c r="A21" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42" t="s">
+      <c r="B21" s="41"/>
+      <c r="C21" s="91" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+    </row>
+    <row r="22" spans="1:6" s="36" customFormat="1" ht="41.1" customHeight="1">
+      <c r="A22" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+    </row>
+    <row r="23" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A23" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+    </row>
+    <row r="24" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A24" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+    </row>
+    <row r="25" spans="1:6" s="36" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+    </row>
+    <row r="26" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A26" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="37" customFormat="1" ht="57" customHeight="1">
+      <c r="A27" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="72"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-    </row>
-    <row r="21" spans="1:6" s="37" customFormat="1" ht="45.95" customHeight="1">
-      <c r="A21" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="93" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-    </row>
-    <row r="22" spans="1:6" s="37" customFormat="1" ht="41.1" customHeight="1">
-      <c r="A22" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="93" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-    </row>
-    <row r="23" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A23" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-    </row>
-    <row r="24" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A24" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-    </row>
-    <row r="25" spans="1:6" s="37" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-    </row>
-    <row r="26" spans="1:6" s="38" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A26" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="38" customFormat="1" ht="57" customHeight="1">
-      <c r="A27" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="75"/>
+      <c r="E27" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1974,8 +1964,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1994,70 +1984,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" customHeight="1">
+      <c r="A2" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-    </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="103" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A3" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A4" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-    </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-    </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="103" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+    </row>
+    <row r="5" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A5" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-    </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="105" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+    </row>
+    <row r="6" spans="1:7" ht="83.25" customHeight="1">
+      <c r="A6" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-    </row>
-    <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="98" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="4"/>
@@ -2066,57 +2056,57 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="G7" s="58" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="88" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="G8" s="86" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="90" t="s">
-        <v>66</v>
+        <v>39</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="22.5" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="60" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="G10" s="106" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2133,19 +2123,19 @@
     </row>
     <row r="13" spans="1:7" ht="25.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -2155,7 +2145,7 @@
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2165,7 +2155,7 @@
     <row r="16" spans="1:7" ht="25.5" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2175,7 +2165,7 @@
     <row r="17" spans="1:15" ht="25.5" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -2185,7 +2175,7 @@
     <row r="18" spans="1:15" ht="25.5" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2194,10 +2184,10 @@
     </row>
     <row r="19" spans="1:15" ht="27.75" customHeight="1">
       <c r="A19" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -2217,215 +2207,215 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="18"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
     </row>
     <row r="23" spans="1:15" ht="42" customHeight="1">
-      <c r="A23" s="99" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
+      <c r="A23" s="101" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="23"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="34"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="3"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
     </row>
     <row r="24" spans="1:15" ht="61.5" customHeight="1">
       <c r="A24" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="100"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
     </row>
     <row r="25" spans="1:15" ht="42" customHeight="1">
-      <c r="A25" s="101" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
+      <c r="A25" s="103" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="3"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
     </row>
     <row r="26" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="99" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="99"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="99"/>
+      <c r="G26" s="99"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+    </row>
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A27" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="97"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="52"/>
-    </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="97" t="s">
+      <c r="B27" s="99"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="51"/>
+    </row>
+    <row r="28" spans="1:15" ht="45" customHeight="1">
+      <c r="E28" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+    </row>
+    <row r="29" spans="1:15" ht="24" customHeight="1">
+      <c r="D29" s="78"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
-    </row>
-    <row r="28" spans="1:15" ht="45" customHeight="1">
-      <c r="E28" s="83" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-    </row>
-    <row r="29" spans="1:15" ht="24" customHeight="1">
-      <c r="D29" s="80"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="81" t="s">
+      <c r="G29" s="80"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+    </row>
+    <row r="30" spans="1:15" ht="69.75" customHeight="1">
+      <c r="D30" s="78"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="80"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+    </row>
+    <row r="31" spans="1:15" ht="42" customHeight="1">
+      <c r="D31" s="78"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="80"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+    </row>
+    <row r="32" spans="1:15" ht="53.1" customHeight="1">
+      <c r="D32" s="78"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="G29" s="82"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="52"/>
-    </row>
-    <row r="30" spans="1:15" ht="69.75" customHeight="1">
-      <c r="D30" s="80"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="82"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-    </row>
-    <row r="31" spans="1:15" ht="42" customHeight="1">
-      <c r="D31" s="80"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="82"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="52"/>
-      <c r="O31" s="52"/>
-    </row>
-    <row r="32" spans="1:15" ht="53.1" customHeight="1">
-      <c r="D32" s="80"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="79"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
+      <c r="G32" s="77"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="51"/>
     </row>
     <row r="33" spans="4:7" ht="27.75" customHeight="1">
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="77"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="75"/>
     </row>
     <row r="34" spans="4:7" ht="27.75" customHeight="1">
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="77"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="75"/>
     </row>
     <row r="35" spans="4:7" ht="27.75" customHeight="1">
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="75"/>
     </row>
     <row r="36" spans="4:7" ht="24.75" customHeight="1">
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="77"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="75"/>
     </row>
     <row r="37" spans="4:7" ht="21" customHeight="1">
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="77"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="75"/>
     </row>
     <row r="38" spans="4:7" ht="21" customHeight="1">
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="77"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="75"/>
     </row>
     <row r="39" spans="4:7" ht="21" customHeight="1">
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="77"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="75"/>
     </row>
     <row r="40" spans="4:7" ht="21" customHeight="1">
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="77"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="75"/>
     </row>
     <row r="41" spans="4:7" ht="21" customHeight="1">
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="77"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="75"/>
     </row>
     <row r="42" spans="4:7" ht="21" customHeight="1">
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="77"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="75"/>
     </row>
     <row r="43" spans="4:7" ht="21" customHeight="1">
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="77"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="75"/>
     </row>
     <row r="44" spans="4:7" ht="21" customHeight="1">
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="77"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="75"/>
     </row>
     <row r="45" spans="4:7" ht="25.5" customHeight="1"/>
     <row r="46" spans="4:7" ht="21" customHeight="1"/>
@@ -2437,17 +2427,17 @@
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -2464,13 +2454,13 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="68" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="66" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="6" width="15" style="2" customWidth="1"/>
@@ -2485,146 +2475,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1">
+      <c r="A2" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-    </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1">
-      <c r="A2" s="103" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+    </row>
+    <row r="3" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A3" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+    </row>
+    <row r="4" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A4" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-    </row>
-    <row r="3" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A3" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-    </row>
-    <row r="4" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A4" s="103" t="s">
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A5" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-    </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A5" s="105" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
     </row>
     <row r="6" spans="1:9" ht="54" customHeight="1">
-      <c r="A6" s="98" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
+      <c r="A6" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="89" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="I7" s="87" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="63" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="87" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="I8" s="85" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1">
       <c r="A9" s="4"/>
-      <c r="B9" s="62" t="s">
-        <v>60</v>
+      <c r="B9" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="90" t="s">
-        <v>66</v>
+        <v>39</v>
+      </c>
+      <c r="I9" s="88" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="22.5" customHeight="1">
       <c r="A10" s="4"/>
-      <c r="B10" s="62" t="s">
-        <v>61</v>
+      <c r="B10" s="60" t="s">
+        <v>60</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="I10" s="107" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="20.25" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="62" t="s">
-        <v>34</v>
+      <c r="B11" s="60" t="s">
+        <v>33</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2633,7 +2623,7 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="62"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
@@ -2644,9 +2634,9 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="62" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="12"/>
@@ -2656,8 +2646,8 @@
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1">
       <c r="A14" s="4"/>
-      <c r="B14" s="65" t="s">
-        <v>62</v>
+      <c r="B14" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -2668,8 +2658,8 @@
     </row>
     <row r="15" spans="1:9" ht="21" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="66" t="s">
-        <v>45</v>
+      <c r="B15" s="64" t="s">
+        <v>44</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2680,8 +2670,8 @@
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1">
       <c r="A16" s="4"/>
-      <c r="B16" s="66" t="s">
-        <v>46</v>
+      <c r="B16" s="64" t="s">
+        <v>45</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2692,8 +2682,8 @@
     </row>
     <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="66" t="s">
-        <v>63</v>
+      <c r="B17" s="64" t="s">
+        <v>62</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -2704,8 +2694,8 @@
     </row>
     <row r="18" spans="1:8" ht="21" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="66" t="s">
-        <v>48</v>
+      <c r="B18" s="64" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2716,23 +2706,23 @@
     </row>
     <row r="19" spans="1:8" ht="27.75" customHeight="1">
       <c r="A19" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="60" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="27.75" customHeight="1">
       <c r="A20" s="20"/>
-      <c r="B20" s="67"/>
+      <c r="B20" s="65"/>
     </row>
     <row r="21" spans="1:8" ht="27.75" customHeight="1">
       <c r="A21" s="20"/>
-      <c r="B21" s="67"/>
+      <c r="B21" s="65"/>
     </row>
     <row r="22" spans="1:8" ht="27.75" customHeight="1">
       <c r="A22" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2744,65 +2734,65 @@
     </row>
     <row r="23" spans="1:8" ht="65.25" customHeight="1">
       <c r="A23" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="106" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="106"/>
-      <c r="D23" s="106"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A24" s="106" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="106"/>
-      <c r="C24" s="106"/>
-      <c r="D24" s="106"/>
+      <c r="A24" s="104" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="104"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
     </row>
     <row r="25" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A25" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
+      <c r="A25" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A26" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
+      <c r="A26" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A27" s="84"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="86"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="84"/>
       <c r="F27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="86"/>
+      <c r="H27" s="84"/>
     </row>
     <row r="28" spans="1:8" ht="27.75" customHeight="1"/>
     <row r="29" spans="1:8" ht="27.75" customHeight="1"/>
@@ -2817,107 +2807,107 @@
     <row r="38" spans="1:9" ht="27.75" customHeight="1"/>
     <row r="39" spans="1:9" ht="27.75" customHeight="1"/>
     <row r="40" spans="1:9" ht="27.75" customHeight="1">
-      <c r="A40" s="73"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
+      <c r="A40" s="71"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
     </row>
     <row r="41" spans="1:9" ht="27.75" customHeight="1">
       <c r="A41" s="21"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
     </row>
     <row r="42" spans="1:9" ht="27.75" customHeight="1">
       <c r="A42" s="21"/>
-      <c r="B42" s="69"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
     </row>
     <row r="43" spans="1:9" ht="27.75" customHeight="1">
       <c r="A43" s="21"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="56"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
     </row>
     <row r="44" spans="1:9" ht="27.75" customHeight="1">
       <c r="A44" s="21"/>
-      <c r="B44" s="69"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
     </row>
     <row r="45" spans="1:9" ht="27.75" customHeight="1">
       <c r="A45" s="21"/>
-      <c r="B45" s="69"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
     </row>
     <row r="46" spans="1:9" ht="27.75" customHeight="1">
       <c r="A46" s="21"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
     </row>
     <row r="47" spans="1:9" ht="27.75" customHeight="1">
       <c r="A47" s="21"/>
-      <c r="B47" s="69"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
     </row>
     <row r="48" spans="1:9" ht="27.75" customHeight="1">
       <c r="A48" s="21"/>
-      <c r="B48" s="69"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
     </row>
     <row r="49" spans="1:9" ht="42" customHeight="1">
       <c r="A49" s="23"/>
-      <c r="B49" s="70"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="24"/>
       <c r="D49" s="23"/>
       <c r="E49" s="25"/>
@@ -2931,7 +2921,7 @@
     <row r="52" spans="1:9" ht="44.1" customHeight="1"/>
     <row r="53" spans="1:9" ht="24.75" customHeight="1"/>
     <row r="54" spans="1:9" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="B54" s="71"/>
+      <c r="B54" s="69"/>
     </row>
     <row r="55" spans="1:9" ht="42" customHeight="1"/>
     <row r="56" spans="1:9" ht="24" customHeight="1"/>

</xml_diff>